<commit_message>
Refine Model & Update docs
</commit_message>
<xml_diff>
--- a/docs/results.xlsx
+++ b/docs/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Home_Working_Status_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Home_Working_Status_Analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A99775-7D65-4465-9EDB-E32401994791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2772C42C-EEF3-404D-B611-2D63D6ECF24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="1470" windowWidth="20595" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1095" yWindow="0" windowWidth="18390" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -177,6 +177,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -184,9 +190,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -471,13 +474,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="30.625" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="3" width="30.625" customWidth="1"/>
+    <col min="4" max="4" width="1.25" customWidth="1"/>
     <col min="5" max="6" width="25.625" customWidth="1"/>
     <col min="7" max="9" width="15.625" customWidth="1"/>
   </cols>
@@ -487,10 +492,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -504,344 +509,390 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C2" s="2">
         <v>16</v>
       </c>
-      <c r="C2" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0.29199999999999998</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.38019999999999998</v>
+      <c r="D2" s="4">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.8901</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.64859999999999995</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.87949999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2">
+        <v>64</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.61009999999999998</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.88570000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C5" s="1">
         <v>16</v>
       </c>
-      <c r="C3" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="D5" s="4">
         <v>0.70750000000000002</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E5" s="4">
         <v>0.86660000000000004</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1">
+    </row>
+    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="1">
         <v>32</v>
       </c>
-      <c r="C4" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.30299999999999999</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0.41110000000000002</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="D6" s="4">
         <v>0.74960000000000004</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E6" s="4">
         <v>0.89319999999999999</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1">
-        <v>64</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.32129999999999997</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0.374</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="1">
         <v>64</v>
       </c>
-      <c r="C7" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="4">
+        <v>0.74209999999999998</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.87890000000000001</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C8" s="2">
         <v>16</v>
       </c>
-      <c r="C8" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="4">
+        <v>0.68320000000000003</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.86480000000000001</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="2">
+        <v>32</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.88439999999999996</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1">
-        <v>32</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.62429999999999997</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.85240000000000005</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1">
-        <v>32</v>
+      <c r="A11" s="6"/>
+      <c r="B11" s="8">
+        <v>1E-4</v>
       </c>
       <c r="C11" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.70230000000000004</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.82679999999999998</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1">
-        <v>64</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="1">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.74580000000000002</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.88019999999999998</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="1">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="1">
         <v>64</v>
       </c>
-      <c r="C13" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="4">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.88100000000000001</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C14" s="2">
         <v>16</v>
       </c>
-      <c r="C14" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="4">
+        <v>0.70240000000000002</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.88019999999999998</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="2">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.66490000000000005</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.88129999999999997</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1">
-        <v>32</v>
-      </c>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.70340000000000003</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.88919999999999999</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="1">
-        <v>32</v>
+      <c r="A17" s="6"/>
+      <c r="B17" s="8">
+        <v>1E-4</v>
       </c>
       <c r="C17" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.68679999999999997</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.84619999999999995</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1">
-        <v>64</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="1">
+        <v>32</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.75019999999999998</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.87080000000000002</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="1">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="1">
         <v>64</v>
       </c>
-      <c r="C19" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="4">
+        <v>0.77110000000000001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.90210000000000001</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C20" s="2">
         <v>16</v>
       </c>
-      <c r="C20" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="4">
+        <v>0.71040000000000003</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.88519999999999999</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="2">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.89800000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="2">
+        <v>64</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.66649999999999998</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.89990000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="C23" s="1">
         <v>16</v>
       </c>
-      <c r="C21" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1">
+      <c r="D23" s="4">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.83679999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="1">
         <v>32</v>
       </c>
-      <c r="C22" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1">
+      <c r="D24" s="4">
+        <v>0.75919999999999999</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="1">
         <v>64</v>
       </c>
-      <c r="C24" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="1">
-        <v>64</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="4">
+        <v>0.77439999999999998</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.91110000000000002</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="12">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>